<commit_message>
Update the K8s Upgrade doc
</commit_message>
<xml_diff>
--- a/Resume_avk/.1DevOps.xlsx
+++ b/Resume_avk/.1DevOps.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="190">
   <si>
     <t>Date</t>
   </si>
@@ -533,27 +533,6 @@
     <t>Jenkins backup</t>
   </si>
   <si>
-    <t>Study</t>
-  </si>
-  <si>
-    <t>Maven, SonarQube</t>
-  </si>
-  <si>
-    <t>Artifactory</t>
-  </si>
-  <si>
-    <t>TRF</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Need to check VPC &amp; S3 &amp; ELB &amp; EC2</t>
-  </si>
-  <si>
     <t>50DQ</t>
   </si>
   <si>
@@ -572,61 +551,43 @@
     <t>Balaji</t>
   </si>
   <si>
-    <t xml:space="preserve">EKS-KALYAN </t>
-  </si>
-  <si>
-    <t>RESUME</t>
-  </si>
-  <si>
-    <t>28, 29, 30</t>
-  </si>
-  <si>
-    <t>1, 2</t>
-  </si>
-  <si>
-    <t>3, 4</t>
-  </si>
-  <si>
-    <t>5, 6, 7</t>
-  </si>
-  <si>
-    <t>IMP Things</t>
-  </si>
-  <si>
-    <t>8, 9 10</t>
-  </si>
-  <si>
-    <t>K8S troubleshooting</t>
-  </si>
-  <si>
-    <t>AWS Ranga till Section 19</t>
-  </si>
-  <si>
-    <t>CKA Course</t>
-  </si>
-  <si>
-    <t>System design by Raj</t>
-  </si>
-  <si>
-    <t>all the files stuff need to write and learn</t>
-  </si>
-  <si>
-    <t>Need to learn all the gitHub</t>
-  </si>
-  <si>
-    <t>DB-N from Docker</t>
-  </si>
-  <si>
-    <t>EKS PD</t>
-  </si>
-  <si>
-    <t>AWS RANGA till Section 19</t>
-  </si>
-  <si>
-    <t>System Design by Raj</t>
-  </si>
-  <si>
-    <t>EKS-Kalyan docker and K8s fundamentals</t>
+    <t>Docker IQS</t>
+  </si>
+  <si>
+    <t>School Start</t>
+  </si>
+  <si>
+    <t>Kids will come/ Resume Upload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented New strategy watch 1 hour, prepare notes, study 1 hour. currently my voice is worst and there is no flow. need to improve a lot. </t>
+  </si>
+  <si>
+    <t>DB-N 10 - 15                          CKA-SC                   CKA-N</t>
+  </si>
+  <si>
+    <t>AWS 1 - 19                 GitHub Projects</t>
+  </si>
+  <si>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>ST-I</t>
+  </si>
+  <si>
+    <t>8 50 DQ</t>
+  </si>
+  <si>
+    <t>6, 7 DIQS</t>
+  </si>
+  <si>
+    <t>Resume &amp; Manifests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision </t>
+  </si>
+  <si>
+    <t>Revision Resume Upload</t>
   </si>
 </sst>
 </file>
@@ -762,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -847,6 +808,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -857,24 +834,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -895,9 +854,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1285,7 +1249,7 @@
       <c r="D3" s="7">
         <v>36</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="33" t="s">
         <v>57</v>
       </c>
       <c r="F3" s="29"/>
@@ -1315,7 +1279,7 @@
       <c r="D4" s="7">
         <v>35</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="29"/>
       <c r="G4" s="27" t="s">
         <v>85</v>
@@ -1343,11 +1307,11 @@
       <c r="D5" s="7">
         <v>34</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="34" t="s">
         <v>86</v>
       </c>
       <c r="I5" t="s">
@@ -1373,9 +1337,9 @@
       <c r="D6" s="1">
         <v>33</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="29"/>
-      <c r="G6" s="39"/>
+      <c r="G6" s="35"/>
       <c r="I6" s="6" t="s">
         <v>144</v>
       </c>
@@ -1399,9 +1363,9 @@
       <c r="D7" s="1">
         <v>32</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="29"/>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="36" t="s">
         <v>87</v>
       </c>
       <c r="I7" t="s">
@@ -1430,9 +1394,9 @@
       <c r="D8" s="1">
         <v>31</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="29"/>
-      <c r="G8" s="40"/>
+      <c r="G8" s="36"/>
       <c r="I8" t="s">
         <v>146</v>
       </c>
@@ -1456,7 +1420,7 @@
       <c r="D9" s="1">
         <v>30</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="29"/>
       <c r="G9" s="10" t="s">
         <v>64</v>
@@ -1484,7 +1448,7 @@
       <c r="D10" s="1">
         <v>29</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F10" s="29"/>
@@ -1514,7 +1478,7 @@
       <c r="D11" s="1">
         <v>28</v>
       </c>
-      <c r="E11" s="36"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="29"/>
       <c r="G11" s="37"/>
       <c r="I11" s="6" t="s">
@@ -1534,7 +1498,7 @@
       <c r="D12" s="1">
         <v>27</v>
       </c>
-      <c r="E12" s="36"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="29"/>
       <c r="G12" s="37" t="s">
         <v>89</v>
@@ -1553,7 +1517,7 @@
       <c r="D13" s="1">
         <v>26</v>
       </c>
-      <c r="E13" s="36"/>
+      <c r="E13" s="33"/>
       <c r="F13" s="29"/>
       <c r="G13" s="37"/>
     </row>
@@ -1570,7 +1534,7 @@
       <c r="D14" s="1">
         <v>25</v>
       </c>
-      <c r="E14" s="36"/>
+      <c r="E14" s="33"/>
       <c r="F14" s="29"/>
       <c r="G14" s="11" t="s">
         <v>66</v>
@@ -1589,7 +1553,7 @@
       <c r="D15" s="1">
         <v>24</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="29"/>
       <c r="G15" s="37" t="s">
         <v>90</v>
@@ -1615,7 +1579,7 @@
       <c r="D16" s="1">
         <v>23</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="29"/>
       <c r="G16" s="37"/>
       <c r="H16" s="14"/>
@@ -1638,7 +1602,7 @@
       <c r="D17" s="1">
         <v>22</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="33" t="s">
         <v>59</v>
       </c>
       <c r="F17" s="29"/>
@@ -1665,7 +1629,7 @@
       <c r="D18" s="1">
         <v>21</v>
       </c>
-      <c r="E18" s="36"/>
+      <c r="E18" s="33"/>
       <c r="F18" s="29"/>
       <c r="G18" s="37"/>
       <c r="H18" s="12" t="s">
@@ -1693,7 +1657,7 @@
       <c r="D19" s="1">
         <v>20</v>
       </c>
-      <c r="E19" s="36"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="29"/>
       <c r="G19" s="37"/>
       <c r="H19" s="37" t="s">
@@ -1717,7 +1681,7 @@
       <c r="D20" s="1">
         <v>19</v>
       </c>
-      <c r="E20" s="36"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="29"/>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
@@ -1740,12 +1704,12 @@
       <c r="D21" s="1">
         <v>18</v>
       </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="33"/>
       <c r="F21" s="29"/>
       <c r="G21" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="35"/>
+      <c r="H21" s="41"/>
       <c r="J21" s="6" t="s">
         <v>158</v>
       </c>
@@ -1765,12 +1729,12 @@
       <c r="D22" s="7">
         <v>17</v>
       </c>
-      <c r="E22" s="36"/>
+      <c r="E22" s="33"/>
       <c r="F22" s="29"/>
-      <c r="G22" s="40" t="s">
+      <c r="G22" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H22" s="35"/>
+      <c r="H22" s="41"/>
       <c r="J22" s="6" t="s">
         <v>159</v>
       </c>
@@ -1790,9 +1754,9 @@
       <c r="D23" s="1">
         <v>16</v>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="29"/>
-      <c r="G23" s="40"/>
+      <c r="G23" s="36"/>
       <c r="J23" s="6" t="s">
         <v>160</v>
       </c>
@@ -1811,11 +1775,11 @@
       <c r="D24" s="1">
         <v>15</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="33" t="s">
         <v>60</v>
       </c>
       <c r="F24" s="29"/>
-      <c r="G24" s="40"/>
+      <c r="G24" s="36"/>
       <c r="J24" s="6" t="s">
         <v>161</v>
       </c>
@@ -1845,7 +1809,7 @@
       <c r="D25" s="1">
         <v>14</v>
       </c>
-      <c r="E25" s="36"/>
+      <c r="E25" s="33"/>
       <c r="F25" s="29"/>
       <c r="G25" s="12" t="s">
         <v>92</v>
@@ -1867,7 +1831,7 @@
       <c r="D26" s="1">
         <v>13</v>
       </c>
-      <c r="E26" s="36"/>
+      <c r="E26" s="33"/>
       <c r="F26" s="29"/>
       <c r="G26" s="11" t="s">
         <v>93</v>
@@ -1890,7 +1854,7 @@
       <c r="D27" s="7">
         <v>12</v>
       </c>
-      <c r="E27" s="36"/>
+      <c r="E27" s="33"/>
       <c r="F27" s="29"/>
       <c r="G27" s="37" t="s">
         <v>95</v>
@@ -1913,7 +1877,7 @@
       <c r="D28" s="1">
         <v>11</v>
       </c>
-      <c r="E28" s="36"/>
+      <c r="E28" s="33"/>
       <c r="F28" s="29"/>
       <c r="G28" s="37"/>
     </row>
@@ -1930,7 +1894,7 @@
       <c r="D29" s="1">
         <v>10</v>
       </c>
-      <c r="E29" s="36"/>
+      <c r="E29" s="33"/>
       <c r="F29" s="29"/>
       <c r="G29" s="37" t="s">
         <v>96</v>
@@ -1949,7 +1913,7 @@
       <c r="D30" s="1">
         <v>9</v>
       </c>
-      <c r="E30" s="36"/>
+      <c r="E30" s="33"/>
       <c r="F30" s="29"/>
       <c r="G30" s="37"/>
       <c r="J30" s="6" t="s">
@@ -1969,7 +1933,7 @@
       <c r="D31" s="1">
         <v>8</v>
       </c>
-      <c r="E31" s="36" t="s">
+      <c r="E31" s="33" t="s">
         <v>62</v>
       </c>
       <c r="F31" s="29"/>
@@ -1991,7 +1955,7 @@
       <c r="D32" s="1">
         <v>7</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="33"/>
       <c r="F32" s="29"/>
       <c r="G32" s="16" t="s">
         <v>64</v>
@@ -2013,8 +1977,8 @@
       <c r="D33" s="1">
         <v>6</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="32" t="s">
+      <c r="E33" s="33"/>
+      <c r="F33" s="38" t="s">
         <v>151</v>
       </c>
       <c r="G33" s="37" t="s">
@@ -2040,8 +2004,8 @@
       <c r="D34" s="1">
         <v>5</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="37"/>
       <c r="H34" s="4" t="s">
         <v>70</v>
@@ -2060,8 +2024,8 @@
       <c r="D35" s="1">
         <v>4</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="37"/>
       <c r="H35" s="4" t="s">
         <v>71</v>
@@ -2080,8 +2044,8 @@
       <c r="D36" s="1">
         <v>3</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="37"/>
       <c r="H36" s="4" t="s">
         <v>72</v>
@@ -2100,8 +2064,8 @@
       <c r="D37" s="1">
         <v>2</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="37"/>
       <c r="H37" s="4" t="s">
         <v>73</v>
@@ -2120,8 +2084,8 @@
       <c r="D38" s="1">
         <v>1</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="40"/>
       <c r="G38" s="37"/>
       <c r="H38" s="4" t="s">
         <v>74</v>
@@ -2347,6 +2311,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F33:F38"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E31:E38"/>
+    <mergeCell ref="G33:G38"/>
+    <mergeCell ref="H19:H20"/>
     <mergeCell ref="E3:E9"/>
     <mergeCell ref="E10:E16"/>
     <mergeCell ref="E17:E23"/>
@@ -2359,11 +2328,6 @@
     <mergeCell ref="G22:G24"/>
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="G29:G31"/>
-    <mergeCell ref="F33:F38"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="E31:E38"/>
-    <mergeCell ref="G33:G38"/>
-    <mergeCell ref="H19:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2372,16 +2336,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X35"/>
+  <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E10"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -2396,712 +2361,558 @@
         <v>3</v>
       </c>
       <c r="D1" s="31"/>
-      <c r="L1" t="s">
-        <v>175</v>
-      </c>
-      <c r="M1" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="29">
-        <v>52</v>
-      </c>
-      <c r="B2" s="3">
-        <v>44706</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="29">
-        <v>33</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>176</v>
-      </c>
-      <c r="R2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V2" t="s">
-        <v>80</v>
-      </c>
-      <c r="X2" s="48">
-        <v>44708</v>
+      <c r="A2" s="7">
+        <v>49</v>
+      </c>
+      <c r="B2" s="8">
+        <v>44709</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <v>30</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3">
-        <v>44707</v>
+        <v>44710</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" s="29">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s">
-        <v>136</v>
-      </c>
-      <c r="L3" t="s">
-        <v>176</v>
-      </c>
-      <c r="R3" t="s">
-        <v>78</v>
-      </c>
-      <c r="V3" t="s">
-        <v>13</v>
-      </c>
-      <c r="X3" s="48">
-        <v>44708</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E3" s="49"/>
+      <c r="J3" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="X3" s="32"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
-        <v>44708</v>
+        <v>44711</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4" s="29">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E4" s="49"/>
-      <c r="F4" t="s">
-        <v>199</v>
-      </c>
-      <c r="K4" t="s">
-        <v>172</v>
-      </c>
-      <c r="R4" t="s">
-        <v>34</v>
-      </c>
-      <c r="V4" t="s">
-        <v>184</v>
-      </c>
-      <c r="X4" s="48">
-        <v>44708</v>
-      </c>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3">
-        <v>44709</v>
+        <v>44712</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" s="29">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="49"/>
-      <c r="F5" t="s">
-        <v>200</v>
+      <c r="J5" s="50" t="s">
+        <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>173</v>
-      </c>
-      <c r="R5" t="s">
-        <v>80</v>
-      </c>
-      <c r="V5" t="s">
-        <v>28</v>
-      </c>
-      <c r="X5" t="s">
-        <v>186</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="X5" s="32"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3">
-        <v>44710</v>
+        <v>44713</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" s="29">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="49"/>
-      <c r="F6" t="s">
-        <v>201</v>
-      </c>
+      <c r="J6" s="50"/>
       <c r="K6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" t="s">
-        <v>176</v>
-      </c>
-      <c r="R6" t="s">
-        <v>81</v>
-      </c>
-      <c r="V6" t="s">
-        <v>178</v>
-      </c>
-      <c r="X6" s="48">
-        <v>44712</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3">
-        <v>44711</v>
+        <v>44714</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" s="29">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7" s="49"/>
-      <c r="F7" t="s">
-        <v>198</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>176</v>
-      </c>
-      <c r="R7" t="s">
-        <v>37</v>
-      </c>
-      <c r="T7" t="s">
-        <v>82</v>
-      </c>
-      <c r="V7" t="s">
-        <v>179</v>
-      </c>
-      <c r="X7" t="s">
-        <v>187</v>
-      </c>
+      <c r="J7" s="50"/>
+      <c r="K7" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="X7" s="32"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3">
-        <v>44712</v>
+        <v>44715</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D8" s="29">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" s="49"/>
-      <c r="F8" t="s">
-        <v>202</v>
-      </c>
-      <c r="K8" t="s">
-        <v>15</v>
-      </c>
-      <c r="R8" t="s">
-        <v>56</v>
-      </c>
-      <c r="V8" t="s">
-        <v>182</v>
-      </c>
-      <c r="X8" s="48">
-        <v>44715</v>
+      <c r="J8" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3">
-        <v>44713</v>
+        <v>44716</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D9" s="29">
-        <v>26</v>
-      </c>
-      <c r="E9" s="49"/>
-      <c r="F9" t="s">
-        <v>194</v>
-      </c>
-      <c r="K9" t="s">
-        <v>17</v>
-      </c>
-      <c r="R9" t="s">
-        <v>28</v>
-      </c>
-      <c r="V9" t="s">
-        <v>180</v>
-      </c>
-      <c r="X9" t="s">
-        <v>188</v>
+        <v>23</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="J9" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3">
-        <v>44714</v>
+        <v>44717</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D10" s="29">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="49"/>
-      <c r="F10" t="s">
-        <v>192</v>
-      </c>
-      <c r="K10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" t="s">
-        <v>177</v>
-      </c>
-      <c r="R10" t="s">
-        <v>83</v>
-      </c>
-      <c r="V10" t="s">
-        <v>181</v>
-      </c>
-      <c r="X10" s="48" t="s">
-        <v>189</v>
+      <c r="J10" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3">
-        <v>44715</v>
+        <v>44718</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D11" s="29">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>196</v>
-      </c>
-      <c r="K11" t="s">
-        <v>174</v>
-      </c>
-      <c r="L11" t="s">
-        <v>176</v>
-      </c>
-      <c r="V11" t="s">
-        <v>183</v>
-      </c>
-      <c r="W11" t="s">
-        <v>190</v>
-      </c>
-      <c r="X11" t="s">
-        <v>191</v>
+        <v>21</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="J11" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3">
-        <v>44716</v>
+        <v>44719</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D12" s="29">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>197</v>
-      </c>
-      <c r="K12" t="s">
-        <v>19</v>
-      </c>
-      <c r="V12" t="s">
-        <v>185</v>
-      </c>
-      <c r="X12">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="E12" s="49"/>
+      <c r="J12" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3">
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D13" s="29">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>83</v>
-      </c>
-      <c r="K13" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="J13" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3">
-        <v>44718</v>
+        <v>44721</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D14" s="29">
-        <v>21</v>
-      </c>
-      <c r="K14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" t="s">
-        <v>176</v>
+        <v>18</v>
+      </c>
+      <c r="E14" s="49"/>
+      <c r="J14" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
-        <v>39</v>
-      </c>
-      <c r="B15" s="3">
-        <v>44719</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="29">
-        <v>20</v>
+      <c r="A15" s="7">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8">
+        <v>44722</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>17</v>
+      </c>
+      <c r="E15" s="49"/>
+      <c r="J15" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3">
-        <v>44720</v>
+        <v>44723</v>
       </c>
       <c r="C16" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="29">
+        <v>16</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3">
+        <v>44724</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="29">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>171</v>
+      </c>
+      <c r="J17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44725</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="29">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>175</v>
+      </c>
+      <c r="J18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3">
+        <v>44726</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="29">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>31</v>
+      </c>
+      <c r="B20" s="8">
+        <v>44727</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D20" s="7">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" t="s">
+        <v>173</v>
+      </c>
+      <c r="J20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="29">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3">
+        <v>44728</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="29">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="29">
+        <v>29</v>
+      </c>
+      <c r="B22" s="3">
+        <v>44729</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="29">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
+        <v>28</v>
+      </c>
+      <c r="B23" s="3">
+        <v>44730</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="29">
+        <v>27</v>
+      </c>
+      <c r="B24" s="3">
+        <v>44731</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <v>26</v>
+      </c>
+      <c r="B25" s="3">
+        <v>44732</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="29">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3">
+        <v>44733</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="29">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3">
+        <v>44734</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="29">
+        <v>23</v>
+      </c>
+      <c r="B28" s="3">
+        <v>44735</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="29">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3">
+        <v>44736</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="29">
+        <v>21</v>
+      </c>
+      <c r="B30" s="3">
+        <v>44737</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="29">
+        <v>20</v>
+      </c>
+      <c r="B31" s="3">
+        <v>44738</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="29">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
-        <v>37</v>
-      </c>
-      <c r="B17" s="3">
-        <v>44721</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="29">
-        <v>18</v>
-      </c>
-      <c r="V17" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>36</v>
-      </c>
-      <c r="B18" s="8">
-        <v>44722</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="7">
-        <v>17</v>
-      </c>
-      <c r="V18" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3">
-        <v>44723</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="29">
-        <v>16</v>
-      </c>
-      <c r="V19" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
-        <v>34</v>
-      </c>
-      <c r="B20" s="3">
-        <v>44724</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="29">
-        <v>15</v>
-      </c>
-      <c r="V20" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
-        <v>33</v>
-      </c>
-      <c r="B21" s="3">
-        <v>44725</v>
-      </c>
-      <c r="C21" s="29" t="s">
+      <c r="B32" s="3">
+        <v>44739</v>
+      </c>
+      <c r="C32" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="29">
-        <v>14</v>
-      </c>
-      <c r="V21" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
-        <v>32</v>
-      </c>
-      <c r="B22" s="3">
-        <v>44726</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="29">
-        <v>13</v>
-      </c>
-      <c r="V22" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>31</v>
-      </c>
-      <c r="B23" s="8">
-        <v>44727</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="7">
-        <v>12</v>
-      </c>
-      <c r="V23" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
-        <v>30</v>
-      </c>
-      <c r="B24" s="3">
-        <v>44728</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="29">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
-        <v>29</v>
-      </c>
-      <c r="B25" s="3">
-        <v>44729</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
-        <v>28</v>
-      </c>
-      <c r="B26" s="3">
-        <v>44730</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="29">
-        <v>27</v>
-      </c>
-      <c r="B27" s="3">
-        <v>44731</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
-        <v>26</v>
-      </c>
-      <c r="B28" s="3">
-        <v>44732</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="29">
-        <v>25</v>
-      </c>
-      <c r="B29" s="3">
-        <v>44733</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
-        <v>24</v>
-      </c>
-      <c r="B30" s="3">
-        <v>44734</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="29">
-        <v>23</v>
-      </c>
-      <c r="B31" s="3">
-        <v>44735</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="29">
-        <v>22</v>
-      </c>
-      <c r="B32" s="3">
-        <v>44736</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>4</v>
-      </c>
       <c r="D32" s="29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
-        <v>21</v>
-      </c>
-      <c r="B33" s="3">
-        <v>44737</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="29">
-        <v>20</v>
-      </c>
-      <c r="B34" s="3">
-        <v>44738</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="29">
-        <v>19</v>
-      </c>
-      <c r="B35" s="3">
-        <v>44739</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="29">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E4:E10"/>
+  <mergeCells count="4">
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E9:E15"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3345,7 +3156,7 @@
       <c r="D10" s="19">
         <v>29</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F10" s="46"/>
@@ -3369,7 +3180,7 @@
       <c r="D11" s="19">
         <v>28</v>
       </c>
-      <c r="E11" s="36"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3385,8 +3196,8 @@
       <c r="D12" s="19">
         <v>27</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="38" t="s">
+      <c r="E12" s="33"/>
+      <c r="F12" s="34" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3403,8 +3214,8 @@
       <c r="D13" s="19">
         <v>26</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="41"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
@@ -3419,8 +3230,8 @@
       <c r="D14" s="19">
         <v>25</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="39"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
@@ -3435,7 +3246,7 @@
       <c r="D15" s="19">
         <v>24</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="45" t="s">
         <v>135</v>
       </c>
@@ -3454,7 +3265,7 @@
       <c r="D16" s="19">
         <v>23</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="47"/>
       <c r="G16" s="21"/>
     </row>
@@ -3471,10 +3282,10 @@
       <c r="D17" s="19">
         <v>22</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="34" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3491,8 +3302,8 @@
       <c r="D18" s="19">
         <v>21</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="39"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
@@ -3507,7 +3318,7 @@
       <c r="D19" s="19">
         <v>20</v>
       </c>
-      <c r="E19" s="36"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="45" t="s">
         <v>137</v>
       </c>
@@ -3525,7 +3336,7 @@
       <c r="D20" s="19">
         <v>19</v>
       </c>
-      <c r="E20" s="36"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3541,11 +3352,11 @@
       <c r="D21" s="19">
         <v>18</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="38" t="s">
+      <c r="E21" s="33"/>
+      <c r="F21" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="35"/>
+      <c r="G21" s="41"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
@@ -3560,9 +3371,9 @@
       <c r="D22" s="7">
         <v>17</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="35"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="41"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
@@ -3577,8 +3388,8 @@
       <c r="D23" s="19">
         <v>16</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="38" t="s">
+      <c r="E23" s="33"/>
+      <c r="F23" s="34" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3595,10 +3406,10 @@
       <c r="D24" s="19">
         <v>15</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="41"/>
+      <c r="F24" s="48"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
@@ -3613,8 +3424,8 @@
       <c r="D25" s="19">
         <v>14</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="39"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="35"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
@@ -3629,8 +3440,8 @@
       <c r="D26" s="19">
         <v>13</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="38" t="s">
+      <c r="E26" s="33"/>
+      <c r="F26" s="34" t="s">
         <v>139</v>
       </c>
       <c r="G26" s="12" t="s">
@@ -3650,8 +3461,8 @@
       <c r="D27" s="7">
         <v>12</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="41"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="48"/>
       <c r="G27" s="12" t="s">
         <v>94</v>
       </c>
@@ -3669,8 +3480,8 @@
       <c r="D28" s="19">
         <v>11</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="48"/>
       <c r="G28" s="37" t="s">
         <v>77</v>
       </c>
@@ -3688,8 +3499,8 @@
       <c r="D29" s="19">
         <v>10</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="41"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="48"/>
       <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3705,8 +3516,8 @@
       <c r="D30" s="19">
         <v>9</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="39"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="35"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
@@ -3721,10 +3532,10 @@
       <c r="D31" s="19">
         <v>8</v>
       </c>
-      <c r="E31" s="36" t="s">
+      <c r="E31" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="38" t="s">
+      <c r="F31" s="34" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3741,8 +3552,8 @@
       <c r="D32" s="19">
         <v>7</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="39"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="35"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
@@ -3757,8 +3568,8 @@
       <c r="D33" s="19">
         <v>6</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="38" t="s">
+      <c r="E33" s="33"/>
+      <c r="F33" s="34" t="s">
         <v>140</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -3778,8 +3589,8 @@
       <c r="D34" s="19">
         <v>5</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="39"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="4" t="s">
         <v>70</v>
       </c>
@@ -3797,8 +3608,8 @@
       <c r="D35" s="19">
         <v>4</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="38" t="s">
+      <c r="E35" s="33"/>
+      <c r="F35" s="34" t="s">
         <v>68</v>
       </c>
       <c r="G35" s="4" t="s">
@@ -3818,8 +3629,8 @@
       <c r="D36" s="19">
         <v>3</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="48"/>
       <c r="G36" s="4" t="s">
         <v>72</v>
       </c>
@@ -3837,8 +3648,8 @@
       <c r="D37" s="19">
         <v>2</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="48"/>
       <c r="G37" s="4" t="s">
         <v>73</v>
       </c>
@@ -3856,8 +3667,8 @@
       <c r="D38" s="19">
         <v>1</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="39"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="35"/>
       <c r="G38" s="4" t="s">
         <v>74</v>
       </c>
@@ -4079,6 +3890,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E31:E38"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="F26:F30"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F35:F38"/>
     <mergeCell ref="E10:E16"/>
     <mergeCell ref="E17:E23"/>
     <mergeCell ref="E5:E9"/>
@@ -4091,12 +3908,6 @@
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="E31:E38"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="F26:F30"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F35:F38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>